<commit_message>
Initial commit with project setup and email generation code
</commit_message>
<xml_diff>
--- a/Data/Student_Emails.xlsx
+++ b/Data/Student_Emails.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2202,6 +2202,1599 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>1</v>
+      </c>
+      <c r="B66" t="n">
+        <v>136603</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Adhiambo, Jane Daisy</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>37684</v>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>adaisy@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2</v>
+      </c>
+      <c r="B67" t="n">
+        <v>142285</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Ali, Sumeiya Abdulle Abdirizak</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>37377</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>aabdirizak@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>3</v>
+      </c>
+      <c r="B68" t="n">
+        <v>146072</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Asava, Wayne Majani</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>37563</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>amajani@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4</v>
+      </c>
+      <c r="B69" t="n">
+        <v>145210</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Barasa, Michelle Nekesa</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>36702</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>bnekesa@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>5</v>
+      </c>
+      <c r="B70" t="n">
+        <v>143496</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Bigingi, Ian Duncan</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>37730</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>bduncan@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>6</v>
+      </c>
+      <c r="B71" t="n">
+        <v>146171</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Cheboi, Lormotum Noel</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>36728</v>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>cnoel@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>7</v>
+      </c>
+      <c r="B72" t="n">
+        <v>145835</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Dulo, Humphrey James</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>37368</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>djames@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>8</v>
+      </c>
+      <c r="B73" t="n">
+        <v>146565</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Etemesi, Caleb Asira</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>37656</v>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>easira@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>9</v>
+      </c>
+      <c r="B74" t="n">
+        <v>136046</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Frances, Ayango</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>37220</v>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>fayango@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>10</v>
+      </c>
+      <c r="B75" t="n">
+        <v>146399</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Gitau, Sandra Wanjiru</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>37632</v>
+      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>gwanjiru@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>11</v>
+      </c>
+      <c r="B76" t="n">
+        <v>146424</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Hassan, Masoud Ali</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>37156</v>
+      </c>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>hali1@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>12</v>
+      </c>
+      <c r="B77" t="n">
+        <v>145279</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Kabui, Michelle Miceere</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>37314</v>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>kmiceere@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>13</v>
+      </c>
+      <c r="B78" t="n">
+        <v>145491</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Kamau, Edinah Nyambura</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>37660</v>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>knyambura@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>14</v>
+      </c>
+      <c r="B79" t="n">
+        <v>137991</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Kamau, Jesse Mbugua</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>37847</v>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>kmbugua@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>15</v>
+      </c>
+      <c r="B80" t="n">
+        <v>146013</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Karani, Amanda Ngendo</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>37613</v>
+      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>kngendo@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>16</v>
+      </c>
+      <c r="B81" t="n">
+        <v>145212</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Kathurima, Ryan Kinoti</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>36644</v>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>kkinoti@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>17</v>
+      </c>
+      <c r="B82" t="n">
+        <v>145802</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Kennedy, Angel Venoliah</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>37250</v>
+      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>kvenoliah@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>18</v>
+      </c>
+      <c r="B83" t="n">
+        <v>136395</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Kiilu, Jeff Kioko</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>37618</v>
+      </c>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>kkioko@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>19</v>
+      </c>
+      <c r="B84" t="n">
+        <v>137503</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Kiiru, Cynthia Everlyn Muthoni</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>37230</v>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>kmuthoni1@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>20</v>
+      </c>
+      <c r="B85" t="n">
+        <v>141690</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Kimani, Alex Mwangi</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>37425</v>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>kmwangi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>21</v>
+      </c>
+      <c r="B86" t="n">
+        <v>128576</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Kinegeni, Terry</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>36869</v>
+      </c>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>kterry@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>22</v>
+      </c>
+      <c r="B87" t="n">
+        <v>145602</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Kyalo, Felicia Mutheu</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>36953</v>
+      </c>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>kmutheu@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>23</v>
+      </c>
+      <c r="B88" t="n">
+        <v>138216</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Leting, Sylvester Kiplagat</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>37970</v>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>lkiplagat@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>24</v>
+      </c>
+      <c r="B89" t="n">
+        <v>139991</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Lihanda, Glen Musa</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>37951</v>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>lmusa@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>25</v>
+      </c>
+      <c r="B90" t="n">
+        <v>144915</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Mahia, Jerome Kamau</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>37951</v>
+      </c>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>mkamau@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>26</v>
+      </c>
+      <c r="B91" t="n">
+        <v>115104</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Mbugua, Nathan Ng'ethe</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>37433</v>
+      </c>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>mngethe@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>27</v>
+      </c>
+      <c r="B92" t="n">
+        <v>139074</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Mbwanga, Emmanuel Chivunira</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>37567</v>
+      </c>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>mchivunira@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>28</v>
+      </c>
+      <c r="B93" t="n">
+        <v>92313</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Moire, Henry Nyakundi</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>37718</v>
+      </c>
+      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>mnyakundi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>29</v>
+      </c>
+      <c r="B94" t="n">
+        <v>129029</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Morara, Keith Matwere</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>36764</v>
+      </c>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>mmatwere@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30</v>
+      </c>
+      <c r="B95" t="n">
+        <v>138583</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Muchiri, Lynn Wairimu</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>37094</v>
+      </c>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>mwairimu@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>31</v>
+      </c>
+      <c r="B96" t="n">
+        <v>144338</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Mugendi, Emmanuel Muthomi</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>36754</v>
+      </c>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>mmuthomi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>32</v>
+      </c>
+      <c r="B97" t="n">
+        <v>140091</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Mukiri, Maryanne Wanjiku</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>36812</v>
+      </c>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>mwanjiku@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>33</v>
+      </c>
+      <c r="B98" t="n">
+        <v>145351</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Mungai, Kihanya</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>36779</v>
+      </c>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>mkihanya@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>34</v>
+      </c>
+      <c r="B99" t="n">
+        <v>145836</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Musyoka, Brian Kioko</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>37447</v>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>mkioko@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>35</v>
+      </c>
+      <c r="B100" t="n">
+        <v>139133</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Mutende, Arabella Fanisheba</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>37382</v>
+      </c>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>mfanisheba@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>36</v>
+      </c>
+      <c r="B101" t="n">
+        <v>145703</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Mutinda, Bryan Lwaya</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>37773</v>
+      </c>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>mlwaya@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>37</v>
+      </c>
+      <c r="B102" t="n">
+        <v>146016</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Mwago, Megan Dette</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>37117</v>
+      </c>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>mdette@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>38</v>
+      </c>
+      <c r="B103" t="n">
+        <v>145041</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Mwai, David King</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>36584</v>
+      </c>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>mking@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>39</v>
+      </c>
+      <c r="B104" t="n">
+        <v>145646</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Nalugala, Venessa Chebukwa</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>37208</v>
+      </c>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>nchebukwa@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>40</v>
+      </c>
+      <c r="B105" t="n">
+        <v>145813</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Ndirangu, Denise Nyambura</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>37598</v>
+      </c>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>nnyambura1@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>41</v>
+      </c>
+      <c r="B106" t="n">
+        <v>139149</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Ngahu, David Gitonga</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>36747</v>
+      </c>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>ngitonga@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>42</v>
+      </c>
+      <c r="B107" t="n">
+        <v>141733</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Ngari, Sifa Gathoni</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>37787</v>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>ngathoni@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>43</v>
+      </c>
+      <c r="B108" t="n">
+        <v>134321</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Nguthiru, Edwin Ndiritu</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>36895</v>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>nndiritu@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>44</v>
+      </c>
+      <c r="B109" t="n">
+        <v>145354</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Nyamosi, Edmond Omwega</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>36993</v>
+      </c>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>nomwega@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>45</v>
+      </c>
+      <c r="B110" t="n">
+        <v>145536</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Nyang'or, Olive Menorah</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>37449</v>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>nmenorah@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>46</v>
+      </c>
+      <c r="B111" t="n">
+        <v>122993</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Omal, Warren</t>
+        </is>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>37810</v>
+      </c>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>owarren@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>47</v>
+      </c>
+      <c r="B112" t="n">
+        <v>145182</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Omondi, Emmanuel Neville</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>37941</v>
+      </c>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>oneville@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>48</v>
+      </c>
+      <c r="B113" t="n">
+        <v>146533</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Omondi, Winfred Achieng</t>
+        </is>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>36695</v>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>oachieng@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>49</v>
+      </c>
+      <c r="B114" t="n">
+        <v>131778</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Otao, Davis Mokora</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>37046</v>
+      </c>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>omokora@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>50</v>
+      </c>
+      <c r="B115" t="n">
+        <v>146202</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Rintaugu, Mugambi Nteere</t>
+        </is>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>36674</v>
+      </c>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>rnteere@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>51</v>
+      </c>
+      <c r="B116" t="n">
+        <v>146413</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Rotich, Mercy Chepngetich</t>
+        </is>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>37812</v>
+      </c>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>rchepngetich@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>52</v>
+      </c>
+      <c r="B117" t="n">
+        <v>146254</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Sehmi, Singh Jeevan</t>
+        </is>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>36915</v>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>sjeevan@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>53</v>
+      </c>
+      <c r="B118" t="n">
+        <v>144914</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Vasani, Aman Upinkumar</t>
+        </is>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>37616</v>
+      </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>vupinkumar@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>54</v>
+      </c>
+      <c r="B119" t="n">
+        <v>135361</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Wafula, Gideon Simiyu</t>
+        </is>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>37970</v>
+      </c>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>wsimiyu@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>55</v>
+      </c>
+      <c r="B120" t="n">
+        <v>145770</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Wahu, Bridget Makena</t>
+        </is>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>37356</v>
+      </c>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>wmakena@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>56</v>
+      </c>
+      <c r="B121" t="n">
+        <v>145369</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Wango, Michael Mundati</t>
+        </is>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>37596</v>
+      </c>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>wmundati@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>57</v>
+      </c>
+      <c r="B122" t="n">
+        <v>137938</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Wangombe, Martin Mwangi</t>
+        </is>
+      </c>
+      <c r="D122" s="2" t="n">
+        <v>37476</v>
+      </c>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>wmwangi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>58</v>
+      </c>
+      <c r="B123" t="n">
+        <v>145838</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Wanyonyi, Brian Newton</t>
+        </is>
+      </c>
+      <c r="D123" s="2" t="n">
+        <v>37304</v>
+      </c>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>wnewton@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>59</v>
+      </c>
+      <c r="B124" t="n">
+        <v>138616</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Wasike, Nicole Jones Nekesa</t>
+        </is>
+      </c>
+      <c r="D124" s="2" t="n">
+        <v>37945</v>
+      </c>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>wnekesa@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>